<commit_message>
Pushing unstaged files to Master
</commit_message>
<xml_diff>
--- a/FrameworkCarehubble/Excel/Data.xlsx
+++ b/FrameworkCarehubble/Excel/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>shahid+257@troontechnologies.comm</t>
+  </si>
+  <si>
+    <t>12345Qwe!@#</t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,9 +400,33 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -404,6 +434,12 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="B6" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>